<commit_message>
split snapshot and release for auto deploying
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/blog.xlsx
+++ b/src/test/resources/data/out/blog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="24">
   <si>
     <t>Résultat</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Élément non utilisé par le robot suite à une erreur précédente.</t>
+  </si>
+  <si>
+    <t>Échec : Ouverture DEMO.</t>
   </si>
 </sst>
 </file>
@@ -93,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +250,66 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -302,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -345,6 +408,18 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,8 +777,8 @@
       <c r="E2" s="7">
         <v>7</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>20</v>
+      <c r="F2" s="52" t="s">
+        <v>23</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -723,8 +798,8 @@
       <c r="E3" s="8">
         <v>10</v>
       </c>
-      <c r="F3" s="39" t="s">
-        <v>20</v>
+      <c r="F3" s="53" t="s">
+        <v>22</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -744,8 +819,8 @@
       <c r="E4" s="8">
         <v>8</v>
       </c>
-      <c r="F4" s="41" t="s">
-        <v>22</v>
+      <c r="F4" s="52" t="s">
+        <v>23</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -765,7 +840,7 @@
       <c r="E5" s="13">
         <v>2</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="53" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="3"/>
@@ -786,8 +861,8 @@
       <c r="E6" s="8">
         <v>9</v>
       </c>
-      <c r="F6" s="39" t="s">
-        <v>20</v>
+      <c r="F6" s="53" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adapt RestDataProvider to multiple scenarii counters
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/blog.xlsx
+++ b/src/test/resources/data/out/blog.xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
+    <workbookView windowHeight="5745" windowWidth="14670" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
-    <sheet name="NoraUi-blog" sheetId="1" r:id="rId1"/>
+    <sheet name="NoraUi-blog" r:id="rId1" sheetId="1"/>
   </sheets>
   <definedNames>
     <definedName name="Motifs">#REF!</definedName>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>Note</t>
   </si>
@@ -77,13 +77,23 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Succès</t>
+  </si>
+  <si>
+    <t>Échec : anonymous is prohibited in demo blog!!</t>
+  </si>
+  <si>
+    <t>Élément ignoré suite à une erreur précédente.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +127,66 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
   </fonts>
   <fills count="5">
@@ -155,30 +225,42 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="27">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
       <color rgb="FF006058"/>
@@ -201,10 +283,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -362,7 +444,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -371,13 +453,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -387,7 +469,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -396,7 +478,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -405,7 +487,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -415,12 +497,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -451,7 +533,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -470,7 +552,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -482,8 +564,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -491,11 +573,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -518,7 +600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -534,10 +616,12 @@
       <c r="E2" s="6">
         <v>7</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="25" t="s">
+        <v>21</v>
+      </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -553,10 +637,12 @@
       <c r="E3" s="7">
         <v>10</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -572,10 +658,12 @@
       <c r="E4" s="7">
         <v>8</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="24" t="s">
+        <v>20</v>
+      </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -583,7 +671,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -599,10 +687,12 @@
       <c r="E6" s="11">
         <v>2</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="24" t="s">
+        <v>20</v>
+      </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -618,121 +708,123 @@
       <c r="E7" s="7">
         <v>9</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="F7" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row ht="14.45" r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row ht="14.45" r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
@@ -757,7 +849,7 @@
       <c r="B48" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed fr scenario but need to update en
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/blog.xlsx
+++ b/src/test/resources/data/out/blog.xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="5745" windowWidth="14670" xWindow="0" yWindow="2445"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
   </bookViews>
   <sheets>
-    <sheet name="NoraUi-blog" r:id="rId1" sheetId="1"/>
+    <sheet name="NoraUi-blog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Motifs">#REF!</definedName>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Note</t>
   </si>
@@ -77,29 +77,13 @@
   </si>
   <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>Succès</t>
-  </si>
-  <si>
-    <t>Échec : anonymous is prohibited in demo blog!!</t>
-  </si>
-  <si>
-    <t>Élément ignoré suite à une erreur précédente.</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>Fail: anonymous is prohibited in demo blog!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,81 +117,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="53"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="53"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="53"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="53"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="53"/>
     </font>
   </fonts>
   <fills count="5">
@@ -246,45 +155,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
       <color rgb="FF006058"/>
@@ -307,10 +201,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -468,7 +362,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -477,13 +371,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -493,7 +387,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -502,7 +396,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -511,7 +405,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -521,12 +415,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -557,7 +451,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -576,7 +470,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -588,20 +482,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -624,7 +518,7 @@
         <v>19</v>
       </c>
     </row>
-    <row ht="14.45" r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -640,12 +534,10 @@
       <c r="E2" s="6">
         <v>7</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>23</v>
-      </c>
+      <c r="F2" s="5"/>
       <c r="G2" s="3"/>
     </row>
-    <row ht="14.45" r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -661,12 +553,10 @@
       <c r="E3" s="7">
         <v>10</v>
       </c>
-      <c r="F3" s="27" t="s">
-        <v>23</v>
-      </c>
+      <c r="F3" s="8"/>
       <c r="G3" s="3"/>
     </row>
-    <row ht="14.45" r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -682,12 +572,10 @@
       <c r="E4" s="7">
         <v>8</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>23</v>
-      </c>
+      <c r="F4" s="8"/>
       <c r="G4" s="4"/>
     </row>
-    <row ht="14.45" r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -695,7 +583,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="4"/>
     </row>
-    <row ht="14.45" r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -711,12 +599,12 @@
       <c r="E6" s="11">
         <v>2</v>
       </c>
-      <c r="F6" s="28" t="s">
-        <v>24</v>
+      <c r="F6" s="12">
+        <v>3</v>
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row ht="14.45" r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -732,123 +620,121 @@
       <c r="E7" s="7">
         <v>9</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="14.45" r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row ht="14.45" r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row ht="14.45" r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row ht="14.45" r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row ht="14.45" r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row ht="14.45" r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row ht="14.45" r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row ht="14.45" r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row ht="14.45" r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row ht="14.45" r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row ht="14.45" r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row ht="14.45" r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row ht="14.45" r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row ht="14.45" r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
-    <row ht="14.45" r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
     </row>
-    <row ht="14.45" r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
     </row>
-    <row ht="14.45" r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row ht="14.45" r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row ht="14.45" r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row ht="14.45" r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row ht="14.45" r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row ht="14.45" r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row ht="14.45" r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
     </row>
-    <row ht="14.45" r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
     </row>
-    <row ht="14.45" r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
     </row>
-    <row ht="14.45" r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
     </row>
-    <row ht="14.45" r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
     </row>
-    <row ht="14.45" r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
     </row>
-    <row ht="14.45" r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
     </row>
-    <row ht="14.45" r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
     </row>
-    <row ht="14.45" r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
     </row>
-    <row ht="14.45" r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
     </row>
-    <row ht="14.45" r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
     </row>
-    <row ht="14.45" r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
@@ -873,7 +759,7 @@
       <c r="B48" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>